<commit_message>
updated daily death dataset
</commit_message>
<xml_diff>
--- a/0306-0612care_home_deaths.xlsx
+++ b/0306-0612care_home_deaths.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24860" windowHeight="10060"/>
+    <workbookView windowWidth="24860" windowHeight="10140"/>
   </bookViews>
   <sheets>
     <sheet name="0306-0612care_home_deaths" sheetId="1" r:id="rId1"/>
@@ -30,10 +30,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -58,6 +58,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -65,9 +73,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -82,15 +96,23 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -114,32 +136,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -150,9 +157,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -174,15 +180,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,31 +209,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -245,139 +365,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -471,6 +471,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -479,156 +488,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -964,13 +964,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A100"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="17.6" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="10.7857142857143"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -986,729 +989,609 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>43896</v>
+        <v>43876</v>
       </c>
       <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>435</v>
-      </c>
-      <c r="D2">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>43897</v>
+        <v>43877</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>388</v>
-      </c>
-      <c r="D3">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>43898</v>
+        <v>43878</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>446</v>
-      </c>
-      <c r="D4">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>43899</v>
+        <v>43879</v>
       </c>
       <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>402</v>
-      </c>
-      <c r="D5">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>43900</v>
+        <v>43880</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>437</v>
-      </c>
-      <c r="D6">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>43901</v>
+        <v>43881</v>
       </c>
       <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>421</v>
-      </c>
-      <c r="D7">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>43902</v>
+        <v>43882</v>
       </c>
       <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>372</v>
-      </c>
-      <c r="D8">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>43903</v>
+        <v>43883</v>
       </c>
       <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>376</v>
-      </c>
-      <c r="D9">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>43904</v>
+        <v>43884</v>
       </c>
       <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>394</v>
-      </c>
-      <c r="D10">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>43905</v>
+        <v>43885</v>
       </c>
       <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>384</v>
-      </c>
-      <c r="D11">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>43906</v>
+        <v>43886</v>
       </c>
       <c r="B12">
-        <v>8</v>
-      </c>
-      <c r="C12">
-        <v>414</v>
-      </c>
-      <c r="D12">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="1">
-        <v>43907</v>
+        <v>43887</v>
       </c>
       <c r="B13">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>417</v>
-      </c>
-      <c r="D13">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="1">
-        <v>43908</v>
+        <v>43888</v>
       </c>
       <c r="B14">
-        <v>10</v>
-      </c>
-      <c r="C14">
-        <v>411</v>
-      </c>
-      <c r="D14">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="1">
-        <v>43909</v>
+        <v>43889</v>
       </c>
       <c r="B15">
-        <v>11</v>
-      </c>
-      <c r="C15">
-        <v>407</v>
-      </c>
-      <c r="D15">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" s="1">
-        <v>43910</v>
+        <v>43890</v>
       </c>
       <c r="B16">
-        <v>17</v>
-      </c>
-      <c r="C16">
-        <v>447</v>
-      </c>
-      <c r="D16">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="1">
-        <v>43911</v>
+        <v>43891</v>
       </c>
       <c r="B17">
-        <v>17</v>
-      </c>
-      <c r="C17">
-        <v>447</v>
-      </c>
-      <c r="D17">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="1">
-        <v>43912</v>
+        <v>43892</v>
       </c>
       <c r="B18">
-        <v>23</v>
-      </c>
-      <c r="C18">
-        <v>436</v>
-      </c>
-      <c r="D18">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="1">
-        <v>43913</v>
+        <v>43893</v>
       </c>
       <c r="B19">
-        <v>26</v>
-      </c>
-      <c r="C19">
-        <v>421</v>
-      </c>
-      <c r="D19">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="1">
-        <v>43914</v>
+        <v>43894</v>
       </c>
       <c r="B20">
-        <v>33</v>
-      </c>
-      <c r="C20">
-        <v>450</v>
-      </c>
-      <c r="D20">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="1">
-        <v>43915</v>
+        <v>43895</v>
       </c>
       <c r="B21">
-        <v>45</v>
-      </c>
-      <c r="C21">
-        <v>499</v>
-      </c>
-      <c r="D21">
-        <v>370</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1">
-        <v>43916</v>
+        <v>43896</v>
       </c>
       <c r="B22">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="C22">
-        <v>550</v>
+        <v>435</v>
       </c>
       <c r="D22">
-        <v>364</v>
+        <v>434</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1">
-        <v>43917</v>
+        <v>43897</v>
       </c>
       <c r="B23">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <v>519</v>
+        <v>388</v>
       </c>
       <c r="D23">
-        <v>373</v>
+        <v>377</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1">
-        <v>43918</v>
+        <v>43898</v>
       </c>
       <c r="B24">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <v>576</v>
+        <v>446</v>
       </c>
       <c r="D24">
-        <v>353</v>
+        <v>374</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1">
-        <v>43919</v>
+        <v>43899</v>
       </c>
       <c r="B25">
-        <v>81</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>493</v>
+        <v>402</v>
       </c>
       <c r="D25">
-        <v>375</v>
+        <v>400</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1">
-        <v>43920</v>
+        <v>43900</v>
       </c>
       <c r="B26">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>622</v>
+        <v>437</v>
       </c>
       <c r="D26">
-        <v>377</v>
+        <v>414</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1">
-        <v>43921</v>
+        <v>43901</v>
       </c>
       <c r="B27">
-        <v>131</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>590</v>
+        <v>421</v>
       </c>
       <c r="D27">
-        <v>330</v>
+        <v>364</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1">
-        <v>43922</v>
+        <v>43902</v>
       </c>
       <c r="B28">
-        <v>151</v>
+        <v>2</v>
       </c>
       <c r="C28">
-        <v>658</v>
+        <v>372</v>
       </c>
       <c r="D28">
-        <v>344</v>
+        <v>419</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1">
-        <v>43923</v>
+        <v>43903</v>
       </c>
       <c r="B29">
-        <v>187</v>
+        <v>3</v>
       </c>
       <c r="C29">
-        <v>643</v>
+        <v>376</v>
       </c>
       <c r="D29">
-        <v>383</v>
+        <v>373</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1">
-        <v>43924</v>
+        <v>43904</v>
       </c>
       <c r="B30">
-        <v>231</v>
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>683</v>
+        <v>394</v>
       </c>
       <c r="D30">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1">
-        <v>43925</v>
+        <v>43905</v>
       </c>
       <c r="B31">
-        <v>236</v>
+        <v>5</v>
       </c>
       <c r="C31">
-        <v>744</v>
+        <v>384</v>
       </c>
       <c r="D31">
-        <v>363</v>
+        <v>373</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1">
-        <v>43926</v>
+        <v>43906</v>
       </c>
       <c r="B32">
-        <v>289</v>
+        <v>8</v>
       </c>
       <c r="C32">
-        <v>740</v>
+        <v>414</v>
       </c>
       <c r="D32">
-        <v>374</v>
+        <v>389</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1">
-        <v>43927</v>
+        <v>43907</v>
       </c>
       <c r="B33">
-        <v>274</v>
+        <v>15</v>
       </c>
       <c r="C33">
-        <v>738</v>
+        <v>417</v>
       </c>
       <c r="D33">
-        <v>373</v>
+        <v>377</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1">
-        <v>43928</v>
+        <v>43908</v>
       </c>
       <c r="B34">
-        <v>357</v>
+        <v>10</v>
       </c>
       <c r="C34">
-        <v>753</v>
+        <v>411</v>
       </c>
       <c r="D34">
-        <v>394</v>
+        <v>368</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1">
-        <v>43929</v>
+        <v>43909</v>
       </c>
       <c r="B35">
-        <v>381</v>
+        <v>11</v>
       </c>
       <c r="C35">
-        <v>777</v>
+        <v>407</v>
       </c>
       <c r="D35">
-        <v>385</v>
+        <v>391</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1">
-        <v>43930</v>
+        <v>43910</v>
       </c>
       <c r="B36">
-        <v>385</v>
+        <v>17</v>
       </c>
       <c r="C36">
-        <v>786</v>
+        <v>447</v>
       </c>
       <c r="D36">
-        <v>405</v>
+        <v>380</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1">
-        <v>43931</v>
+        <v>43911</v>
       </c>
       <c r="B37">
-        <v>403</v>
+        <v>17</v>
       </c>
       <c r="C37">
-        <v>809</v>
+        <v>447</v>
       </c>
       <c r="D37">
-        <v>373</v>
+        <v>378</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1">
-        <v>43932</v>
+        <v>43912</v>
       </c>
       <c r="B38">
-        <v>447</v>
+        <v>23</v>
       </c>
       <c r="C38">
-        <v>810</v>
+        <v>436</v>
       </c>
       <c r="D38">
-        <v>375</v>
+        <v>350</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1">
-        <v>43933</v>
+        <v>43913</v>
       </c>
       <c r="B39">
-        <v>495</v>
+        <v>26</v>
       </c>
       <c r="C39">
-        <v>805</v>
+        <v>421</v>
       </c>
       <c r="D39">
-        <v>407</v>
+        <v>340</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1">
-        <v>43934</v>
+        <v>43914</v>
       </c>
       <c r="B40">
-        <v>414</v>
+        <v>33</v>
       </c>
       <c r="C40">
-        <v>694</v>
+        <v>450</v>
       </c>
       <c r="D40">
-        <v>379</v>
+        <v>330</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1">
-        <v>43935</v>
+        <v>43915</v>
       </c>
       <c r="B41">
-        <v>453</v>
+        <v>45</v>
       </c>
       <c r="C41">
-        <v>630</v>
+        <v>499</v>
       </c>
       <c r="D41">
-        <v>358</v>
+        <v>370</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1">
-        <v>43936</v>
+        <v>43916</v>
       </c>
       <c r="B42">
-        <v>466</v>
+        <v>45</v>
       </c>
       <c r="C42">
-        <v>720</v>
+        <v>550</v>
       </c>
       <c r="D42">
-        <v>401</v>
+        <v>364</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1">
-        <v>43937</v>
+        <v>43917</v>
       </c>
       <c r="B43">
-        <v>526</v>
+        <v>64</v>
       </c>
       <c r="C43">
-        <v>755</v>
+        <v>519</v>
       </c>
       <c r="D43">
-        <v>411</v>
+        <v>373</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1">
-        <v>43938</v>
+        <v>43918</v>
       </c>
       <c r="B44">
-        <v>540</v>
+        <v>67</v>
       </c>
       <c r="C44">
-        <v>666</v>
+        <v>576</v>
       </c>
       <c r="D44">
-        <v>391</v>
+        <v>353</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1">
-        <v>43939</v>
+        <v>43919</v>
       </c>
       <c r="B45">
-        <v>499</v>
+        <v>81</v>
       </c>
       <c r="C45">
-        <v>650</v>
+        <v>493</v>
       </c>
       <c r="D45">
-        <v>428</v>
+        <v>375</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1">
-        <v>43940</v>
+        <v>43920</v>
       </c>
       <c r="B46">
-        <v>470</v>
+        <v>107</v>
       </c>
       <c r="C46">
-        <v>655</v>
+        <v>622</v>
       </c>
       <c r="D46">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="1">
-        <v>43941</v>
+        <v>43921</v>
       </c>
       <c r="B47">
-        <v>480</v>
+        <v>131</v>
       </c>
       <c r="C47">
-        <v>638</v>
+        <v>590</v>
       </c>
       <c r="D47">
-        <v>351</v>
+        <v>330</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1">
-        <v>43942</v>
+        <v>43922</v>
       </c>
       <c r="B48">
-        <v>436</v>
+        <v>151</v>
       </c>
       <c r="C48">
-        <v>640</v>
+        <v>658</v>
       </c>
       <c r="D48">
-        <v>377</v>
+        <v>344</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1">
-        <v>43943</v>
+        <v>43923</v>
       </c>
       <c r="B49">
-        <v>492</v>
+        <v>187</v>
       </c>
       <c r="C49">
-        <v>593</v>
+        <v>643</v>
       </c>
       <c r="D49">
-        <v>343</v>
+        <v>383</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1">
-        <v>43944</v>
+        <v>43924</v>
       </c>
       <c r="B50">
-        <v>458</v>
+        <v>231</v>
       </c>
       <c r="C50">
-        <v>599</v>
+        <v>683</v>
       </c>
       <c r="D50">
-        <v>364</v>
+        <v>403</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1">
-        <v>43945</v>
+        <v>43925</v>
       </c>
       <c r="B51">
-        <v>454</v>
+        <v>236</v>
       </c>
       <c r="C51">
-        <v>573</v>
+        <v>744</v>
       </c>
       <c r="D51">
-        <v>356</v>
+        <v>363</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1">
-        <v>43946</v>
+        <v>43926</v>
       </c>
       <c r="B52">
-        <v>444</v>
+        <v>289</v>
       </c>
       <c r="C52">
-        <v>586</v>
+        <v>740</v>
       </c>
       <c r="D52">
-        <v>351</v>
+        <v>374</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1">
-        <v>43947</v>
+        <v>43927</v>
       </c>
       <c r="B53">
-        <v>402</v>
+        <v>274</v>
       </c>
       <c r="C53">
-        <v>533</v>
+        <v>738</v>
       </c>
       <c r="D53">
         <v>373</v>
@@ -1716,475 +1599,475 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="1">
-        <v>43948</v>
+        <v>43928</v>
       </c>
       <c r="B54">
-        <v>389</v>
+        <v>357</v>
       </c>
       <c r="C54">
-        <v>553</v>
+        <v>753</v>
       </c>
       <c r="D54">
-        <v>365</v>
+        <v>394</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="1">
-        <v>43949</v>
+        <v>43929</v>
       </c>
       <c r="B55">
+        <v>381</v>
+      </c>
+      <c r="C55">
+        <v>777</v>
+      </c>
+      <c r="D55">
         <v>385</v>
-      </c>
-      <c r="C55">
-        <v>436</v>
-      </c>
-      <c r="D55">
-        <v>353</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="1">
-        <v>43950</v>
+        <v>43930</v>
       </c>
       <c r="B56">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="C56">
-        <v>456</v>
+        <v>786</v>
       </c>
       <c r="D56">
-        <v>349</v>
+        <v>405</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="1">
-        <v>43951</v>
+        <v>43931</v>
       </c>
       <c r="B57">
-        <v>336</v>
+        <v>403</v>
       </c>
       <c r="C57">
-        <v>474</v>
+        <v>809</v>
       </c>
       <c r="D57">
-        <v>380</v>
+        <v>373</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="1">
-        <v>43952</v>
+        <v>43932</v>
       </c>
       <c r="B58">
-        <v>356</v>
+        <v>447</v>
       </c>
       <c r="C58">
-        <v>491</v>
+        <v>810</v>
       </c>
       <c r="D58">
-        <v>385</v>
+        <v>375</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1">
-        <v>43953</v>
+        <v>43933</v>
       </c>
       <c r="B59">
-        <v>331</v>
+        <v>495</v>
       </c>
       <c r="C59">
-        <v>444</v>
+        <v>805</v>
       </c>
       <c r="D59">
-        <v>307</v>
+        <v>407</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1">
-        <v>43954</v>
+        <v>43934</v>
       </c>
       <c r="B60">
-        <v>312</v>
+        <v>414</v>
       </c>
       <c r="C60">
-        <v>421</v>
+        <v>694</v>
       </c>
       <c r="D60">
-        <v>326</v>
+        <v>379</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="1">
-        <v>43955</v>
+        <v>43935</v>
       </c>
       <c r="B61">
-        <v>308</v>
+        <v>453</v>
       </c>
       <c r="C61">
-        <v>445</v>
+        <v>630</v>
       </c>
       <c r="D61">
-        <v>306</v>
+        <v>358</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="1">
-        <v>43956</v>
+        <v>43936</v>
       </c>
       <c r="B62">
-        <v>295</v>
+        <v>466</v>
       </c>
       <c r="C62">
-        <v>364</v>
+        <v>720</v>
       </c>
       <c r="D62">
-        <v>341</v>
+        <v>401</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="1">
-        <v>43957</v>
+        <v>43937</v>
       </c>
       <c r="B63">
-        <v>267</v>
+        <v>526</v>
       </c>
       <c r="C63">
-        <v>377</v>
+        <v>755</v>
       </c>
       <c r="D63">
-        <v>324</v>
+        <v>411</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="1">
-        <v>43958</v>
+        <v>43938</v>
       </c>
       <c r="B64">
-        <v>292</v>
+        <v>540</v>
       </c>
       <c r="C64">
-        <v>387</v>
+        <v>666</v>
       </c>
       <c r="D64">
-        <v>344</v>
+        <v>391</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="1">
-        <v>43959</v>
+        <v>43939</v>
       </c>
       <c r="B65">
-        <v>274</v>
+        <v>499</v>
       </c>
       <c r="C65">
-        <v>416</v>
+        <v>650</v>
       </c>
       <c r="D65">
-        <v>335</v>
+        <v>428</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="1">
-        <v>43960</v>
+        <v>43940</v>
       </c>
       <c r="B66">
-        <v>287</v>
+        <v>470</v>
       </c>
       <c r="C66">
-        <v>392</v>
+        <v>655</v>
       </c>
       <c r="D66">
-        <v>363</v>
+        <v>379</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="1">
-        <v>43961</v>
+        <v>43941</v>
       </c>
       <c r="B67">
-        <v>224</v>
+        <v>480</v>
       </c>
       <c r="C67">
-        <v>338</v>
+        <v>638</v>
       </c>
       <c r="D67">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="1">
-        <v>43962</v>
+        <v>43942</v>
       </c>
       <c r="B68">
-        <v>184</v>
+        <v>436</v>
       </c>
       <c r="C68">
-        <v>313</v>
+        <v>640</v>
       </c>
       <c r="D68">
-        <v>347</v>
+        <v>377</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="1">
-        <v>43963</v>
+        <v>43943</v>
       </c>
       <c r="B69">
-        <v>201</v>
+        <v>492</v>
       </c>
       <c r="C69">
-        <v>302</v>
+        <v>593</v>
       </c>
       <c r="D69">
-        <v>329</v>
+        <v>343</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="1">
-        <v>43964</v>
+        <v>43944</v>
       </c>
       <c r="B70">
-        <v>213</v>
+        <v>458</v>
       </c>
       <c r="C70">
-        <v>327</v>
+        <v>599</v>
       </c>
       <c r="D70">
-        <v>335</v>
+        <v>364</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="1">
-        <v>43965</v>
+        <v>43945</v>
       </c>
       <c r="B71">
-        <v>208</v>
+        <v>454</v>
       </c>
       <c r="C71">
-        <v>304</v>
+        <v>573</v>
       </c>
       <c r="D71">
-        <v>365</v>
+        <v>356</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="1">
-        <v>43966</v>
+        <v>43946</v>
       </c>
       <c r="B72">
-        <v>197</v>
+        <v>444</v>
       </c>
       <c r="C72">
-        <v>356</v>
+        <v>586</v>
       </c>
       <c r="D72">
-        <v>359</v>
+        <v>351</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="1">
-        <v>43967</v>
+        <v>43947</v>
       </c>
       <c r="B73">
-        <v>202</v>
+        <v>402</v>
       </c>
       <c r="C73">
-        <v>332</v>
+        <v>533</v>
       </c>
       <c r="D73">
-        <v>336</v>
+        <v>373</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="1">
-        <v>43968</v>
+        <v>43948</v>
       </c>
       <c r="B74">
-        <v>171</v>
+        <v>389</v>
       </c>
       <c r="C74">
-        <v>356</v>
+        <v>553</v>
       </c>
       <c r="D74">
-        <v>318</v>
+        <v>365</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="1">
-        <v>43969</v>
+        <v>43949</v>
       </c>
       <c r="B75">
-        <v>179</v>
+        <v>385</v>
       </c>
       <c r="C75">
-        <v>312</v>
+        <v>436</v>
       </c>
       <c r="D75">
-        <v>363</v>
+        <v>353</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="1">
-        <v>43970</v>
+        <v>43950</v>
       </c>
       <c r="B76">
-        <v>162</v>
+        <v>392</v>
       </c>
       <c r="C76">
-        <v>314</v>
+        <v>456</v>
       </c>
       <c r="D76">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="1">
-        <v>43971</v>
+        <v>43951</v>
       </c>
       <c r="B77">
-        <v>143</v>
+        <v>336</v>
       </c>
       <c r="C77">
-        <v>328</v>
+        <v>474</v>
       </c>
       <c r="D77">
-        <v>376</v>
+        <v>380</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="1">
-        <v>43972</v>
+        <v>43952</v>
       </c>
       <c r="B78">
-        <v>135</v>
+        <v>356</v>
       </c>
       <c r="C78">
-        <v>328</v>
+        <v>491</v>
       </c>
       <c r="D78">
-        <v>327</v>
+        <v>385</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="1">
-        <v>43973</v>
+        <v>43953</v>
       </c>
       <c r="B79">
-        <v>130</v>
+        <v>331</v>
       </c>
       <c r="C79">
-        <v>308</v>
+        <v>444</v>
       </c>
       <c r="D79">
-        <v>320</v>
+        <v>307</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="1">
-        <v>43974</v>
+        <v>43954</v>
       </c>
       <c r="B80">
-        <v>123</v>
+        <v>312</v>
       </c>
       <c r="C80">
-        <v>276</v>
+        <v>421</v>
       </c>
       <c r="D80">
-        <v>340</v>
+        <v>326</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="1">
-        <v>43975</v>
+        <v>43955</v>
       </c>
       <c r="B81">
-        <v>120</v>
+        <v>308</v>
       </c>
       <c r="C81">
-        <v>290</v>
+        <v>445</v>
       </c>
       <c r="D81">
-        <v>365</v>
+        <v>306</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="1">
-        <v>43976</v>
+        <v>43956</v>
       </c>
       <c r="B82">
-        <v>109</v>
+        <v>295</v>
       </c>
       <c r="C82">
-        <v>297</v>
+        <v>364</v>
       </c>
       <c r="D82">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="1">
-        <v>43977</v>
+        <v>43957</v>
       </c>
       <c r="B83">
-        <v>134</v>
+        <v>267</v>
       </c>
       <c r="C83">
-        <v>283</v>
+        <v>377</v>
       </c>
       <c r="D83">
-        <v>362</v>
+        <v>324</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="1">
-        <v>43978</v>
+        <v>43958</v>
       </c>
       <c r="B84">
-        <v>111</v>
+        <v>292</v>
       </c>
       <c r="C84">
-        <v>279</v>
+        <v>387</v>
       </c>
       <c r="D84">
-        <v>323</v>
+        <v>344</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="1">
-        <v>43979</v>
+        <v>43959</v>
       </c>
       <c r="B85">
-        <v>120</v>
+        <v>274</v>
       </c>
       <c r="C85">
-        <v>225</v>
+        <v>416</v>
       </c>
       <c r="D85">
-        <v>319</v>
+        <v>335</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="1">
-        <v>43980</v>
+        <v>43960</v>
       </c>
       <c r="B86">
-        <v>94</v>
+        <v>287</v>
       </c>
       <c r="C86">
-        <v>276</v>
+        <v>392</v>
       </c>
       <c r="D86">
-        <v>318</v>
+        <v>363</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="1">
-        <v>43981</v>
+        <v>43961</v>
       </c>
       <c r="B87">
-        <v>83</v>
+        <v>224</v>
       </c>
       <c r="C87">
-        <v>274</v>
+        <v>338</v>
       </c>
       <c r="D87">
         <v>348</v>
@@ -2192,183 +2075,463 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="1">
-        <v>43982</v>
+        <v>43962</v>
       </c>
       <c r="B88">
-        <v>86</v>
+        <v>184</v>
       </c>
       <c r="C88">
-        <v>271</v>
+        <v>313</v>
       </c>
       <c r="D88">
-        <v>321</v>
+        <v>347</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="1">
-        <v>43983</v>
+        <v>43963</v>
       </c>
       <c r="B89">
-        <v>89</v>
+        <v>201</v>
       </c>
       <c r="C89">
-        <v>291</v>
+        <v>302</v>
       </c>
       <c r="D89">
-        <v>338</v>
+        <v>329</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="1">
-        <v>43984</v>
+        <v>43964</v>
       </c>
       <c r="B90">
-        <v>92</v>
+        <v>213</v>
       </c>
       <c r="C90">
-        <v>301</v>
+        <v>327</v>
       </c>
       <c r="D90">
-        <v>365</v>
+        <v>335</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="1">
-        <v>43985</v>
+        <v>43965</v>
       </c>
       <c r="B91">
-        <v>73</v>
+        <v>208</v>
       </c>
       <c r="C91">
-        <v>247</v>
+        <v>304</v>
       </c>
       <c r="D91">
-        <v>302</v>
+        <v>365</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="1">
-        <v>43986</v>
+        <v>43966</v>
       </c>
       <c r="B92">
-        <v>80</v>
+        <v>197</v>
       </c>
       <c r="C92">
-        <v>239</v>
+        <v>356</v>
       </c>
       <c r="D92">
-        <v>336</v>
+        <v>359</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="1">
-        <v>43987</v>
+        <v>43967</v>
       </c>
       <c r="B93">
-        <v>76</v>
+        <v>202</v>
       </c>
       <c r="C93">
-        <v>273</v>
+        <v>332</v>
       </c>
       <c r="D93">
-        <v>318</v>
+        <v>336</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="1">
-        <v>43988</v>
+        <v>43968</v>
       </c>
       <c r="B94">
-        <v>39</v>
+        <v>171</v>
       </c>
       <c r="C94">
-        <v>273</v>
+        <v>356</v>
       </c>
       <c r="D94">
-        <v>313</v>
+        <v>318</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="1">
-        <v>43989</v>
+        <v>43969</v>
       </c>
       <c r="B95">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C95">
-        <v>267</v>
+        <v>312</v>
       </c>
       <c r="D95">
-        <v>320</v>
+        <v>363</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="1">
-        <v>43990</v>
+        <v>43970</v>
       </c>
       <c r="B96">
-        <v>58</v>
+        <v>162</v>
       </c>
       <c r="C96">
-        <v>290</v>
+        <v>314</v>
       </c>
       <c r="D96">
-        <v>317</v>
+        <v>353</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="1">
-        <v>43991</v>
+        <v>43971</v>
       </c>
       <c r="B97">
-        <v>48</v>
+        <v>143</v>
       </c>
       <c r="C97">
-        <v>242</v>
+        <v>328</v>
       </c>
       <c r="D97">
-        <v>308</v>
+        <v>376</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="1">
-        <v>43992</v>
+        <v>43972</v>
       </c>
       <c r="B98">
-        <v>57</v>
+        <v>135</v>
       </c>
       <c r="C98">
-        <v>266</v>
+        <v>328</v>
       </c>
       <c r="D98">
-        <v>314</v>
+        <v>327</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="1">
-        <v>43993</v>
+        <v>43973</v>
       </c>
       <c r="B99">
-        <v>46</v>
+        <v>130</v>
       </c>
       <c r="C99">
-        <v>229</v>
+        <v>308</v>
       </c>
       <c r="D99">
-        <v>304</v>
+        <v>320</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="1">
+        <v>43974</v>
+      </c>
+      <c r="B100">
+        <v>123</v>
+      </c>
+      <c r="C100">
+        <v>276</v>
+      </c>
+      <c r="D100">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="1">
+        <v>43975</v>
+      </c>
+      <c r="B101">
+        <v>120</v>
+      </c>
+      <c r="C101">
+        <v>290</v>
+      </c>
+      <c r="D101">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="1">
+        <v>43976</v>
+      </c>
+      <c r="B102">
+        <v>109</v>
+      </c>
+      <c r="C102">
+        <v>297</v>
+      </c>
+      <c r="D102">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="1">
+        <v>43977</v>
+      </c>
+      <c r="B103">
+        <v>134</v>
+      </c>
+      <c r="C103">
+        <v>283</v>
+      </c>
+      <c r="D103">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="1">
+        <v>43978</v>
+      </c>
+      <c r="B104">
+        <v>111</v>
+      </c>
+      <c r="C104">
+        <v>279</v>
+      </c>
+      <c r="D104">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="1">
+        <v>43979</v>
+      </c>
+      <c r="B105">
+        <v>120</v>
+      </c>
+      <c r="C105">
+        <v>225</v>
+      </c>
+      <c r="D105">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="1">
+        <v>43980</v>
+      </c>
+      <c r="B106">
+        <v>94</v>
+      </c>
+      <c r="C106">
+        <v>276</v>
+      </c>
+      <c r="D106">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="1">
+        <v>43981</v>
+      </c>
+      <c r="B107">
+        <v>83</v>
+      </c>
+      <c r="C107">
+        <v>274</v>
+      </c>
+      <c r="D107">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="1">
+        <v>43982</v>
+      </c>
+      <c r="B108">
+        <v>86</v>
+      </c>
+      <c r="C108">
+        <v>271</v>
+      </c>
+      <c r="D108">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B109">
+        <v>89</v>
+      </c>
+      <c r="C109">
+        <v>291</v>
+      </c>
+      <c r="D109">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="1">
+        <v>43984</v>
+      </c>
+      <c r="B110">
+        <v>92</v>
+      </c>
+      <c r="C110">
+        <v>301</v>
+      </c>
+      <c r="D110">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="1">
+        <v>43985</v>
+      </c>
+      <c r="B111">
+        <v>73</v>
+      </c>
+      <c r="C111">
+        <v>247</v>
+      </c>
+      <c r="D111">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="1">
+        <v>43986</v>
+      </c>
+      <c r="B112">
+        <v>80</v>
+      </c>
+      <c r="C112">
+        <v>239</v>
+      </c>
+      <c r="D112">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="1">
+        <v>43987</v>
+      </c>
+      <c r="B113">
+        <v>76</v>
+      </c>
+      <c r="C113">
+        <v>273</v>
+      </c>
+      <c r="D113">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="1">
+        <v>43988</v>
+      </c>
+      <c r="B114">
+        <v>39</v>
+      </c>
+      <c r="C114">
+        <v>273</v>
+      </c>
+      <c r="D114">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="1">
+        <v>43989</v>
+      </c>
+      <c r="B115">
+        <v>57</v>
+      </c>
+      <c r="C115">
+        <v>267</v>
+      </c>
+      <c r="D115">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="1">
+        <v>43990</v>
+      </c>
+      <c r="B116">
+        <v>58</v>
+      </c>
+      <c r="C116">
+        <v>290</v>
+      </c>
+      <c r="D116">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="1">
+        <v>43991</v>
+      </c>
+      <c r="B117">
+        <v>48</v>
+      </c>
+      <c r="C117">
+        <v>242</v>
+      </c>
+      <c r="D117">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="1">
+        <v>43992</v>
+      </c>
+      <c r="B118">
+        <v>57</v>
+      </c>
+      <c r="C118">
+        <v>266</v>
+      </c>
+      <c r="D118">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="1">
+        <v>43993</v>
+      </c>
+      <c r="B119">
+        <v>46</v>
+      </c>
+      <c r="C119">
+        <v>229</v>
+      </c>
+      <c r="D119">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="1">
         <v>43994</v>
       </c>
-      <c r="B100">
+      <c r="B120">
         <v>41</v>
       </c>
-      <c r="C100">
+      <c r="C120">
         <v>241</v>
       </c>
-      <c r="D100">
+      <c r="D120">
         <v>334</v>
       </c>
     </row>

</xml_diff>